<commit_message>
Edit SDD GUI section
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/week5/Xiaoshan_Week5_Timesheet.xlsx
+++ b/Documentation/TimeSheets/week5/Xiaoshan_Week5_Timesheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyuyangshe/Desktop/2017-S2-SEP-PG29/Documentation/TimeSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\issaclee\Desktop\SEP\2017-S2-SEP-PG29\Documentation\TimeSheets\week5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="20740" windowHeight="11760"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time Sheet" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,16 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Time Sheet'!$6:$6</definedName>
     <definedName name="WorkweekHours">'Time Sheet'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -130,13 +130,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +182,41 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -259,55 +294,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="39" fontId="4" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="39" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Date" xfId="6"/>
+    <cellStyle name="Date" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hours" xfId="7"/>
+    <cellStyle name="Hours" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Phone" xfId="9"/>
-    <cellStyle name="Time" xfId="8"/>
+    <cellStyle name="Phone" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Time" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
@@ -380,7 +415,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Time Sheet" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Time Sheet" pivot="0" count="4">
+    <tableStyle name="Time Sheet" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="4"/>
       <tableStyleElement type="headerRow" dxfId="3"/>
       <tableStyleElement type="firstRowStripe" dxfId="2"/>
@@ -399,14 +434,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TimeSheet" displayName="TimeSheet" ref="B6:F12" totalsRowShown="0">
-  <autoFilter ref="B6:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TimeSheet" displayName="TimeSheet" ref="B6:F12" totalsRowShown="0">
+  <autoFilter ref="B6:F12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="3" name="Activity" dataDxfId="0" dataCellStyle="Date"/>
-    <tableColumn id="1" name="Date(s)" dataCellStyle="Date"/>
-    <tableColumn id="2" name="Time In" dataCellStyle="Time"/>
-    <tableColumn id="5" name="Time Out" dataCellStyle="Time"/>
-    <tableColumn id="6" name="Hours Worked" dataCellStyle="Hours">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Activity" dataDxfId="0" dataCellStyle="Date"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date(s)" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Time In" dataCellStyle="Time"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Out" dataCellStyle="Time"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Hours Worked" dataCellStyle="Hours">
       <calculatedColumnFormula>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-#REF!+#REF!-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -681,28 +716,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="45.5" customWidth="1"/>
-    <col min="3" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" style="2" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.6328125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.7">
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
@@ -713,223 +749,223 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="8">
         <v>10.5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="8">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
         <v>10.5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="8">
         <f>IFERROR(IF(C5&lt;=WorkweekHours,C5,WorkweekHours),"")</f>
         <v>10.5</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="8">
         <f>IFERROR(C5-D5, "")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6" t="s">
+    <row r="7" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="12">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-#REF!+#REF!-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="10">
         <v>42969</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="10">
         <v>42969</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="12">
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="10">
         <v>42971</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="12">
         <v>1</v>
       </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="21">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 F1:XFD5 A2:A1048576 B7:F1048576 G6:XFD1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Time Out in this column under this heading" sqref="E6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hours Worked are automatically calculated in this column under this heading" sqref="F6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Period Start Date in this cell" sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Period End Date in this cell" sqref="C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Total Work Week Hours in cell below" sqref="B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Hours Worked are automatically calculated in cell below" sqref="C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Regular Hours are automatically calculated in cell below" sqref="D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overtime Hours are automatically calculated in cell below" sqref="E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Total Work Week Hours in this cell" sqref="B5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Hours Worked are automatically calculated in this cell" sqref="C5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Regular Hours are automatically calculated in this cell" sqref="D5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overtime Hours are automatically calculated in this cell" sqref="E5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading. Use heading filters to find specific entries" sqref="B6:C6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Time In in this column under this heading" sqref="D6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this worksheet to track hours worked in a work week. Enter Date and Times in TimeSheet table. Total Hours, Regular Hours and Overtime Hours are automatically calculated" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell.  Enter Employee and Manager details in cells below" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Name, Email and Phone in cells at right" sqref="B2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Name in this cell" sqref="C2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Email in this cell" sqref="D2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Phone in this cell" sqref="E2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 F1:XFD5 A2:A1048576 B7:F1048576 G6:XFD1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Time Out in this column under this heading" sqref="E6" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hours Worked are automatically calculated in this column under this heading" sqref="F6" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Period Start Date in this cell" sqref="B3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Period End Date in this cell" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Total Work Week Hours in cell below" sqref="B4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Hours Worked are automatically calculated in cell below" sqref="C4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Regular Hours are automatically calculated in cell below" sqref="D4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overtime Hours are automatically calculated in cell below" sqref="E4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Total Work Week Hours in this cell" sqref="B5" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Hours Worked are automatically calculated in this cell" sqref="C5" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Regular Hours are automatically calculated in this cell" sqref="D5" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overtime Hours are automatically calculated in this cell" sqref="E5" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading. Use heading filters to find specific entries" sqref="B6:C6" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Time In in this column under this heading" sqref="D6" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this worksheet to track hours worked in a work week. Enter Date and Times in TimeSheet table. Total Hours, Regular Hours and Overtime Hours are automatically calculated" sqref="A1" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell.  Enter Employee and Manager details in cells below" sqref="B1" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Name, Email and Phone in cells at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Name in this cell" sqref="C2" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Email in this cell" sqref="D2" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Phone in this cell" sqref="E2" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>

</xml_diff>